<commit_message>
Test the protocol redirect adjustments
</commit_message>
<xml_diff>
--- a/tests/Fixtures/import_redirects.xlsx
+++ b/tests/Fixtures/import_redirects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jyrki/Sites/codedor/filament-redirects/tests/Fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibautdegezelle/Herd/filament-redirects/tests/Fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB8FFFA-2C76-1C43-A4AF-57C0F1BEFC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90B5483-3512-A64F-A51C-C92DDA1B8E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,17 +44,17 @@
     <t>status</t>
   </si>
   <si>
-    <t>/from</t>
+    <t>https://example.com/from</t>
   </si>
   <si>
-    <t>/to</t>
+    <t>https://example.com/to</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -63,6 +63,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -84,15 +91,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -397,7 +407,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -420,10 +430,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2">
@@ -431,6 +441,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5C5C4BA4-FC3D-434F-BDB5-64BF96466546}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C56B40E6-9DF1-7046-BA96-F55EFBB3DDFE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
Feature/fil001 141 redirect url validation (#15)
* Add url validation rules

* Redirect regardless of protocol of url

* Test the protocol redirect adjustments
</commit_message>
<xml_diff>
--- a/tests/Fixtures/import_redirects.xlsx
+++ b/tests/Fixtures/import_redirects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jyrki/Sites/codedor/filament-redirects/tests/Fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibautdegezelle/Herd/filament-redirects/tests/Fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB8FFFA-2C76-1C43-A4AF-57C0F1BEFC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90B5483-3512-A64F-A51C-C92DDA1B8E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,17 +44,17 @@
     <t>status</t>
   </si>
   <si>
-    <t>/from</t>
+    <t>https://example.com/from</t>
   </si>
   <si>
-    <t>/to</t>
+    <t>https://example.com/to</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -63,6 +63,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -84,15 +91,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -397,7 +407,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -420,10 +430,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2">
@@ -431,6 +441,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5C5C4BA4-FC3D-434F-BDB5-64BF96466546}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C56B40E6-9DF1-7046-BA96-F55EFBB3DDFE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>